<commit_message>
Work on Hera EEPROM parameters
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuky\Desktop\hera_python_utility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Admesy_debugging_utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8805B94-F6A5-4548-B715-4E44D469A898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCFB15C-5902-4B5A-96E7-C735335E2785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="41180" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="2750" windowWidth="32890" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -664,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -803,43 +803,37 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1125,7 +1119,7 @@
   <dimension ref="B1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1141,47 +1135,47 @@
   <sheetData>
     <row r="1" spans="2:7" ht="35.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
     </row>
     <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:7" s="3" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="58" t="s">
+      <c r="D4" s="56"/>
+      <c r="E4" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="59"/>
-      <c r="G4" s="60" t="s">
+      <c r="F4" s="56"/>
+      <c r="G4" s="57" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="61"/>
-      <c r="C5" s="62" t="s">
+      <c r="B5" s="60"/>
+      <c r="C5" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="62" t="s">
+      <c r="E5" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="63" t="s">
+      <c r="F5" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="64"/>
+      <c r="G5" s="58"/>
     </row>
     <row r="6" spans="2:7" ht="3.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="15"/>
@@ -1314,7 +1308,7 @@
       <c r="C13" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1388,7 +1382,7 @@
       <c r="C17" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="8" t="s">
@@ -1618,11 +1612,11 @@
     <row r="6" spans="4:8" s="36" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D6" s="46"/>
       <c r="E6" s="47"/>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="54"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="62"/>
     </row>
     <row r="7" spans="4:8" s="36" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D7" s="48"/>

</xml_diff>

<commit_message>
Hera interf almost done
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Admesy_debugging_utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99607345-85A8-4EB3-A798-3FDBBAD34308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9513A06D-A517-4A3D-AAD8-58EF961D14F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13520" yWindow="2440" windowWidth="25730" windowHeight="17920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="41180" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t>Adj. min</t>
   </si>
@@ -200,10 +200,6 @@
   </si>
   <si>
     <t>Why is only a write command?</t>
-  </si>
-  <si>
-    <t>Parameters in the manual are wrong, correct is 0/1
-Why is only a write command?</t>
   </si>
   <si>
     <t>Writes to EEPROM</t>
@@ -283,6 +279,19 @@
   <si>
     <t>EEPROM command is not documented in manual
 :SENSe:SP:INT works also...</t>
+  </si>
+  <si>
+    <t>:SENSe:CAL?</t>
+  </si>
+  <si>
+    <t>:SENSe:CAL Calibration</t>
+  </si>
+  <si>
+    <t>NOT IMPLEMENTED</t>
+  </si>
+  <si>
+    <t>Parameters in the manual for :EEPROM:CONFigure:SPSBW are wrong, correct is 0/1
+Why is only a write command? :SENSe:SP:SBW uses off/user or 0/1 ??</t>
   </si>
 </sst>
 </file>
@@ -331,14 +340,6 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="26"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -347,6 +348,14 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -713,9 +722,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -725,7 +731,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -761,7 +767,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -813,7 +819,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -838,6 +844,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1122,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1139,47 +1148,47 @@
   <sheetData>
     <row r="1" spans="2:7" ht="35.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
     </row>
     <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:7" s="3" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="55" t="s">
+      <c r="D4" s="55"/>
+      <c r="E4" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="57" t="s">
+      <c r="F4" s="55"/>
+      <c r="G4" s="56" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="60"/>
-      <c r="C5" s="52" t="s">
+      <c r="B5" s="59"/>
+      <c r="C5" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="58"/>
+      <c r="G5" s="57"/>
     </row>
     <row r="6" spans="2:7" ht="3.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="15"/>
@@ -1226,7 +1235,7 @@
         <v>49</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="41" customHeight="1" x14ac:dyDescent="0.35">
@@ -1253,11 +1262,11 @@
       <c r="B10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>51</v>
+      <c r="C10" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>74</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>13</v>
@@ -1271,11 +1280,11 @@
       <c r="B11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>51</v>
+      <c r="C11" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>74</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>15</v>
@@ -1289,11 +1298,11 @@
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>51</v>
+      <c r="C12" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="62" t="s">
+        <v>74</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>14</v>
@@ -1309,8 +1318,8 @@
       <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>51</v>
+      <c r="C13" s="62" t="s">
+        <v>74</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>41</v>
@@ -1347,11 +1356,11 @@
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>51</v>
+      <c r="C15" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="62" t="s">
+        <v>74</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>24</v>
@@ -1365,11 +1374,11 @@
       <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>51</v>
+      <c r="C16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>22</v>
@@ -1383,8 +1392,8 @@
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>51</v>
+      <c r="C17" s="62" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>42</v>
@@ -1396,7 +1405,7 @@
         <v>31</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
@@ -1435,154 +1444,154 @@
   <sheetData>
     <row r="1" spans="2:5" ht="35.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="22" t="s">
-        <v>62</v>
+      <c r="B2" s="21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:5" s="3" customFormat="1" ht="50.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="E4" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="5" spans="2:5" ht="3.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="28"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="29"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="24" t="s">
+    </row>
+    <row r="10" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="25" t="s">
+      <c r="D10" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="31" t="s">
+      <c r="E13" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="26" t="s">
+    <row r="14" spans="2:5" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D14" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1613,63 +1622,63 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="4:8" s="36" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D6" s="46"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="61" t="s">
+    <row r="6" spans="4:8" s="35" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="60"/>
+      <c r="H6" s="61"/>
+    </row>
+    <row r="7" spans="4:8" s="35" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="49"/>
+      <c r="H7" s="50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="37"/>
+      <c r="H8" s="44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="61"/>
-      <c r="H6" s="62"/>
-    </row>
-    <row r="7" spans="4:8" s="36" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="51" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="4:8" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="37"/>
-      <c r="F8" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="45" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="4:8" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="39" t="s">
+      <c r="G9" s="37"/>
+      <c r="H9" s="44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D10" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="45" t="s">
+      <c r="E10" s="40"/>
+      <c r="F10" s="41" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="4:8" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D10" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="44" t="s">
-        <v>71</v>
+      <c r="G10" s="42"/>
+      <c r="H10" s="43" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>